<commit_message>
generate year by no invent
</commit_message>
<xml_diff>
--- a/generated_excel/1_Mampang_Information_and_Technology_Riska_Mawardi_1assets.xlsx
+++ b/generated_excel/1_Mampang_Information_and_Technology_Riska_Mawardi_1assets.xlsx
@@ -909,7 +909,11 @@
         </is>
       </c>
       <c r="D9" s="8" t="n"/>
-      <c r="E9" s="9" t="n"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
       <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Riska Mawardi</t>
@@ -917,10 +921,14 @@
       </c>
       <c r="G9" s="9" t="inlineStr">
         <is>
-          <t>Junior Application Developer</t>
-        </is>
-      </c>
-      <c r="H9" s="8" t="n"/>
+          <t>Junior App Dev</t>
+        </is>
+      </c>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Masih Digunakan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n"/>

</xml_diff>